<commit_message>
"parser.xml" -> Anpassungen für lioe-website übernommen. XLSX Dateien aktualisiert. fix #74
</commit_message>
<xml_diff>
--- a/static/Literaturliste_Belegsätze_und_Sekundärliteratur_WBÖ_gesamt.xlsx
+++ b/static/Literaturliste_Belegsätze_und_Sekundärliteratur_WBÖ_gesamt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14412"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14410"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="451">
   <si>
     <t>Kürzel</t>
   </si>
@@ -1264,9 +1264,6 @@
     <t>DRG1975VI</t>
   </si>
   <si>
-    <t>DRG 1975 IV</t>
-  </si>
-  <si>
     <t>Dicziunari Rumantsch Grischun</t>
   </si>
   <si>
@@ -1295,6 +1292,129 @@
   </si>
   <si>
     <t>Wörterbuch zur oberösterreichischen Volksmundart. 8. unveränderte Auflage. Ried im Innkreis 2014</t>
+  </si>
+  <si>
+    <t>Schabus1971I</t>
+  </si>
+  <si>
+    <t>Schabus 1971 I</t>
+  </si>
+  <si>
+    <t>Schabus1971II</t>
+  </si>
+  <si>
+    <t>Schabus 1971 II</t>
+  </si>
+  <si>
+    <t>Dialektgeographie des Lesachtals (Kärnten) - 1</t>
+  </si>
+  <si>
+    <t>Dialektgeographie des Lesachtals (Kärnten) - 2</t>
+  </si>
+  <si>
+    <t>Schabus</t>
+  </si>
+  <si>
+    <t>DRG 1975 VI</t>
+  </si>
+  <si>
+    <t>Pirchegger1927</t>
+  </si>
+  <si>
+    <t>Pirchegger 1927</t>
+  </si>
+  <si>
+    <t>Die slavischen Ortsnamen im Mürzgebiet</t>
+  </si>
+  <si>
+    <t>Pirchegger</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Kronen_Ztg</t>
+  </si>
+  <si>
+    <t>Kronen Zeitung</t>
+  </si>
+  <si>
+    <t>Kronen Zeitung 28.9.1980</t>
+  </si>
+  <si>
+    <t>Krippenspiele aus Oberösterreich und Tirol</t>
+  </si>
+  <si>
+    <t>Pailler1883II</t>
+  </si>
+  <si>
+    <t>Pailler1881I</t>
+  </si>
+  <si>
+    <t>Pailler 1883 II</t>
+  </si>
+  <si>
+    <t>Pailler 1881 I</t>
+  </si>
+  <si>
+    <t>Weihnachtlieder aus Oberösterreich</t>
+  </si>
+  <si>
+    <t>Pailler</t>
+  </si>
+  <si>
+    <t>Wilhelm</t>
+  </si>
+  <si>
+    <t>Schatzdorfer1949</t>
+  </si>
+  <si>
+    <t>Schatzdorfer 1949</t>
+  </si>
+  <si>
+    <t>Spatzngsang und Spinnáwittn</t>
+  </si>
+  <si>
+    <t>Schatzdorfer</t>
+  </si>
+  <si>
+    <t>Goldbacher1904</t>
+  </si>
+  <si>
+    <t>Goldbacher 1904</t>
+  </si>
+  <si>
+    <t>Gmüatlichö Sach'n</t>
+  </si>
+  <si>
+    <t>Goldbacher</t>
+  </si>
+  <si>
+    <t>Gregor</t>
+  </si>
+  <si>
+    <t>DerSchlern1920</t>
+  </si>
+  <si>
+    <t>Der Schlern 1920</t>
+  </si>
+  <si>
+    <t>Bozner Halbmonatsschrift</t>
+  </si>
+  <si>
+    <t>Rudl1920</t>
+  </si>
+  <si>
+    <t>Rudl 1920</t>
+  </si>
+  <si>
+    <t>Rudl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otto  </t>
+  </si>
+  <si>
+    <t>Der Hiesl ban Zonndoktr. Der Schlern. Ausgabe vom 1.6.1920</t>
   </si>
 </sst>
 </file>
@@ -1540,8 +1660,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H99" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:H99"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H109" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:H109"/>
   <sortState ref="A2:H97">
     <sortCondition ref="A1:A97"/>
   </sortState>
@@ -1825,24 +1945,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="150.6640625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" customWidth="1"/>
-    <col min="6" max="6" width="60.6640625" customWidth="1"/>
-    <col min="7" max="7" width="90.44140625" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.08984375" customWidth="1"/>
+    <col min="3" max="3" width="23.36328125" customWidth="1"/>
+    <col min="4" max="4" width="150.6328125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="34.90625" customWidth="1"/>
+    <col min="6" max="6" width="60.6328125" customWidth="1"/>
+    <col min="7" max="7" width="90.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
@@ -1868,7 +1988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>297</v>
       </c>
@@ -1890,7 +2010,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>298</v>
       </c>
@@ -1908,7 +2028,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1927,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>299</v>
       </c>
@@ -1944,7 +2064,7 @@
       <c r="F5" s="9"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>300</v>
       </c>
@@ -1961,7 +2081,7 @@
       <c r="F6" s="9"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>301</v>
       </c>
@@ -1980,7 +2100,7 @@
       <c r="F7" s="9"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -2000,7 +2120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>327</v>
       </c>
@@ -2104,16 +2224,16 @@
         <v>399</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>400</v>
+        <v>417</v>
       </c>
       <c r="C14" s="3">
         <v>1975</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>401</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>402</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -2283,16 +2403,16 @@
     </row>
     <row r="24" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>403</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>404</v>
       </c>
       <c r="C24" s="3">
         <v>1951</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>57</v>
@@ -3736,22 +3856,214 @@
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C99" s="3">
         <v>2014</v>
       </c>
       <c r="D99" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="E99" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>408</v>
+      <c r="B100" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C100" s="3">
+        <v>1971</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C101" s="3">
+        <v>1971</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C102" s="3">
+        <v>1927</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="C103" s="3">
+        <v>1980</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+    </row>
+    <row r="104" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C104" s="3">
+        <v>1883</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="C105" s="3">
+        <v>1881</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C106" s="3">
+        <v>1949</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="C107" s="3">
+        <v>1904</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="C108" s="3">
+        <v>1920</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+    </row>
+    <row r="109" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="C109" s="3">
+        <v>1920</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>